<commit_message>
clarifying biochemical network example
</commit_message>
<xml_diff>
--- a/examples/biochemical_network/data.xlsx
+++ b/examples/biochemical_network/data.xlsx
@@ -12,7 +12,7 @@
     <sheet name="!!Reaction" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'!!Compound'!$A$3:$E$8</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'!!Compound'!$A$3:$D$8</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'!!Reaction'!$A$2:$F$4</definedName>
   </definedNames>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -20,12 +20,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="34">
-  <si>
-    <t>!!!ObjTables objTablesVersion='1.0.1' date='2020-07-07 21:29:38'</t>
-  </si>
-  <si>
-    <t>!!ObjTables type='Data' tableFormat='row' class='Compound' name='Compound' description='Compound' date='2020-03-10 22:56:34' objTablesVersion='1.0.1'</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="33">
+  <si>
+    <t>!!!ObjTables objTablesVersion='1.0.9' date='2020-07-07 21:29:38'</t>
+  </si>
+  <si>
+    <t>!!ObjTables type='Data' tableFormat='row' class='Compound' name='Compound' description='Compound' date='2020-03-10 22:56:34' objTablesVersion='1.0.9'</t>
   </si>
   <si>
     <t>!Model</t>
@@ -40,9 +40,6 @@
     <t>!Identifiers</t>
   </si>
   <si>
-    <t>!IsConstant</t>
-  </si>
-  <si>
     <t>e_coli</t>
   </si>
   <si>
@@ -85,10 +82,10 @@
     <t>kegg.compound:C00022</t>
   </si>
   <si>
-    <t>!!ObjTables type='Data' tableFormat='column' class='Model' name='Model' description='Model' date='2020-03-10 22:56:35' objTablesVersion='1.0.1'</t>
-  </si>
-  <si>
-    <t>!!ObjTables type='Data' tableFormat='row' class='Reaction' name='Reaction' description='Reaction' date='2020-03-10 22:56:35' objTablesVersion='1.0.1'</t>
+    <t>!!ObjTables type='Data' tableFormat='column' class='Model' name='Model' description='Model' date='2020-03-10 22:56:35' objTablesVersion='1.0.9'</t>
+  </si>
+  <si>
+    <t>!!ObjTables type='Data' tableFormat='row' class='Reaction' name='Reaction' description='Reaction' date='2020-03-10 22:56:35' objTablesVersion='1.0.9'</t>
   </si>
   <si>
     <t>!Equation</t>
@@ -185,7 +182,7 @@
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -488,7 +485,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
@@ -497,29 +494,27 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.01" customHeight="1" zeroHeight="1"/>
   <cols>
-    <col min="1" max="5" width="15.7109375" customWidth="1"/>
-    <col min="6" max="16384" width="0" hidden="1" customWidth="1"/>
+    <col min="1" max="4" width="15.7109375" customWidth="1"/>
+    <col min="5" max="16384" width="0" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.01" customHeight="1">
+    <row r="1" spans="1:4" ht="15.01" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-    </row>
-    <row r="2" spans="1:5" ht="15.01" customHeight="1">
+    </row>
+    <row r="2" spans="1:4" ht="15.01" customHeight="1">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-    </row>
-    <row r="3" spans="1:5" ht="15.01" customHeight="1">
+    </row>
+    <row r="3" spans="1:4" ht="15.01" customHeight="1">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
@@ -532,99 +527,81 @@
       <c r="D3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="2" t="s">
+    </row>
+    <row r="4" spans="1:4" ht="15.01" customHeight="1">
+      <c r="A4" s="3" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" ht="15.01" customHeight="1">
-      <c r="A4" s="3" t="s">
+      <c r="B4" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="C4" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="D4" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="3" t="s">
+    </row>
+    <row r="5" spans="1:4" ht="15.01" customHeight="1">
+      <c r="A5" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="E4" s="3" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="15.01" customHeight="1">
-      <c r="A5" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" s="3" t="s">
+      <c r="C5" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="D5" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D5" s="3" t="s">
+    </row>
+    <row r="6" spans="1:4" ht="15.01" customHeight="1">
+      <c r="A6" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="E5" s="3" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="15.01" customHeight="1">
-      <c r="A6" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6" s="3" t="s">
+      <c r="C6" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="D6" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D6" s="3" t="s">
+    </row>
+    <row r="7" spans="1:4" ht="15.01" customHeight="1">
+      <c r="A7" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="E6" s="3" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="15.01" customHeight="1">
-      <c r="A7" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7" s="3" t="s">
+      <c r="C7" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D7" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C7" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="D7" s="3" t="s">
+    </row>
+    <row r="8" spans="1:4" ht="15.01" customHeight="1">
+      <c r="A8" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="E7" s="3" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="15.01" customHeight="1">
-      <c r="A8" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B8" s="3" t="s">
+      <c r="C8" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D8" s="3" t="s">
         <v>19</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="E8" s="3" t="b">
-        <v>1</v>
       </c>
     </row>
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1" insertRows="0" deleteRows="0"/>
-  <autoFilter ref="A3:E8"/>
-  <dataValidations count="5">
+  <autoFilter ref="A3:D8"/>
+  <dataValidations count="4">
     <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Model" error="Value must be a value from &quot;!!Model:2&quot; or blank." promptTitle="Model" prompt="Select a value from &quot;!!Model:2&quot; or blank." sqref="A4:A8">
       <formula1>'!!Model'!$B$2:$XFD$2</formula1>
     </dataValidation>
@@ -637,9 +614,6 @@
     </dataValidation>
     <dataValidation type="textLength" operator="lessThanOrEqual" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Identifiers" error="Value must be a string.&#10;&#10;Value must be less than or equal to 255 characters." promptTitle="Identifiers" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 255 characters." sqref="D4:D8">
       <formula1>255</formula1>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="IsConstant" error="Value must be &quot;True&quot; or &quot;False&quot;." promptTitle="IsConstant" prompt="Select &quot;True&quot; or &quot;False&quot;." sqref="E4:E8">
-      <formula1>"True,False"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -665,7 +639,7 @@
   <sheetData>
     <row r="1" spans="1:2" ht="15.01" customHeight="1">
       <c r="A1" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B1" s="1"/>
     </row>
@@ -674,7 +648,7 @@
         <v>3</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -709,7 +683,7 @@
   <sheetData>
     <row r="1" spans="1:6" ht="15.01" customHeight="1">
       <c r="A1" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -728,53 +702,53 @@
         <v>5</v>
       </c>
       <c r="D2" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="F2" s="2" t="s">
         <v>24</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="15.01" customHeight="1">
       <c r="A3" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B3" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="D3" s="3" t="s">
         <v>27</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>28</v>
       </c>
       <c r="E3" s="3" t="b">
         <v>1</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="15.01" customHeight="1">
       <c r="A4" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B4" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C4" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="D4" s="3" t="s">
         <v>31</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>32</v>
       </c>
       <c r="E4" s="3" t="b">
         <v>1</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>